<commit_message>
feat: add CID-10 selector and data pipeline
</commit_message>
<xml_diff>
--- a/DATA/CID-10.xlsx
+++ b/DATA/CID-10.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,127 +428,303 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>A90</v>
+        <v>A03</v>
       </c>
       <c r="B4" t="str">
-        <v>Dengue [dengue clássico]</v>
+        <v>Shiguelose</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>B50</v>
+        <v>A04</v>
       </c>
       <c r="B5" t="str">
-        <v>Malária por Plasmodium falciparum</v>
+        <v>Outras infecções intestinais bacterianas</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>B54</v>
+        <v>A09</v>
       </c>
       <c r="B6" t="str">
-        <v>Malária não especificada</v>
+        <v>Diarréia e gastroenterite de origem infecciosa presumível</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>J11</v>
+        <v>A90</v>
       </c>
       <c r="B7" t="str">
-        <v>Influenza devida a vírus não identificado</v>
+        <v>Dengue [dengue clássico]</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>J18.9</v>
+        <v>B50</v>
       </c>
       <c r="B8" t="str">
-        <v>Pneumonia não especificada</v>
+        <v>Malária por Plasmodium falciparum</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>J45</v>
+        <v>B54</v>
       </c>
       <c r="B9" t="str">
-        <v>Asma</v>
+        <v>Malária não especificada</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>K29.7</v>
+        <v>B34.2</v>
       </c>
       <c r="B10" t="str">
-        <v>Gastrite não especificada</v>
+        <v>Infecção por coronavírus de localização não especificada</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>M54.5</v>
+        <v>J00</v>
       </c>
       <c r="B11" t="str">
-        <v>Dor lombar baixa</v>
+        <v>Nasofaringite aguda [resfriado comum]</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>R51</v>
+        <v>J01</v>
       </c>
       <c r="B12" t="str">
-        <v>Cefaléia</v>
+        <v>Sinusite aguda</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>S82</v>
+        <v>J02</v>
       </c>
       <c r="B13" t="str">
-        <v>Fratura da perna, incluindo tornozelo</v>
+        <v>Faringite aguda</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Z00.0</v>
+        <v>J03</v>
       </c>
       <c r="B14" t="str">
-        <v>Exame geral e investigação de pessoas sem queixas ou diagnóstico relatado</v>
+        <v>Amigdalite aguda</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>I10</v>
+        <v>J06</v>
       </c>
       <c r="B15" t="str">
-        <v>Hipertensão essencial (primária)</v>
+        <v>Infecções agudas das vias aéreas superiores</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>E11</v>
+        <v>J10</v>
       </c>
       <c r="B16" t="str">
-        <v>Diabetes mellitus não-insulino-dependente</v>
+        <v>Influenza devida a vírus da influenza identificado</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>F32</v>
+        <v>J11</v>
       </c>
       <c r="B17" t="str">
-        <v>Episódios depressivos</v>
+        <v>Influenza devida a vírus não identificado</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
+        <v>J12</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Pneumonia viral</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>J18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Pneumonia por microorganismo não especificado</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>J18.9</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Pneumonia não especificada</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>J20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Bronquite aguda</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>J44</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Outras doenças pulmonares obstrutivas crônicas</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>J45</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Asma</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>I10</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Hipertensão essencial (primária)</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>I20</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Angina pectoris</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>I21</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Infarto agudo do miocárdio</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>I50</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Insuficiência cardíaca</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>E10</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Diabetes mellitus insulino-dependente</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>E11</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Diabetes mellitus não-insulino-dependente</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>E66</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Obesidade</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>F32</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Episódios depressivos</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
         <v>F41</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B32" t="str">
         <v>Outros transtornos ansiosos</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>M54</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Dorsalgia</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>M54.5</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Dor lombar baixa</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>R50</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Febre de outra origem e de origem desconhecida</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>R51</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Cefaléia</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>R52</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Dor não classificada em outra parte</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>S82</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Fratura da perna, incluindo tornozelo</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Z00.0</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Exame geral e investigação de pessoas sem queixas ou diagnóstico relatado</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Z76</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Pessoas em contato com serviços de saúde em outras circunstâncias</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B40"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>